<commit_message>
Prepare table for tableau
</commit_message>
<xml_diff>
--- a/Eisenba/Outputs/Model_Reports.xlsx
+++ b/Eisenba/Outputs/Model_Reports.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,22 +8,23 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Matt\GitHome\Project3\Eisenba\Outputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{4A48488F-C76E-46D2-A161-84D2A76A307D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C52CB32-24EF-4492-9BAE-79B92DD454C0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14355" yWindow="2835" windowWidth="28800" windowHeight="15435"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="28800" windowHeight="15435" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Big_Sheet" sheetId="4" r:id="rId1"/>
-    <sheet name="ExtremeTrees" sheetId="1" r:id="rId2"/>
-    <sheet name="GBoost" sheetId="2" r:id="rId3"/>
-    <sheet name="RandomTrees" sheetId="3" r:id="rId4"/>
+    <sheet name="Scores" sheetId="5" r:id="rId2"/>
+    <sheet name="ExtremeTrees" sheetId="1" r:id="rId3"/>
+    <sheet name="GBoost" sheetId="2" r:id="rId4"/>
+    <sheet name="RandomTrees" sheetId="3" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="15">
   <si>
     <t>precision</t>
   </si>
@@ -63,11 +64,17 @@
   <si>
     <t>Gradient Boost</t>
   </si>
+  <si>
+    <t>Multi-Linear Regression</t>
+  </si>
+  <si>
+    <t>Score</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -901,11 +908,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1236,7 +1243,65 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42057204-692A-4ED9-833B-A25EF06CDE54}">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2">
+        <v>0.77400000000000002</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3">
+        <v>0.63600000000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4">
+        <v>0.76800000000000002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5">
+        <v>0.17499999999999999</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1367,8 +1432,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1499,8 +1564,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
Adds copy for analysis
</commit_message>
<xml_diff>
--- a/Eisenba/Outputs/Model_Reports.xlsx
+++ b/Eisenba/Outputs/Model_Reports.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Matt\GitHome\Project3\Eisenba\Outputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C52CB32-24EF-4492-9BAE-79B92DD454C0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDF6C684-F17D-40D6-92D9-97A21EDAC089}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="28800" windowHeight="15435" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4005" yWindow="2490" windowWidth="28800" windowHeight="15435" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Big_Sheet" sheetId="4" r:id="rId1"/>
@@ -1246,7 +1246,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42057204-692A-4ED9-833B-A25EF06CDE54}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
@@ -1436,11 +1436,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:F6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="16" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B1" t="s">

</xml_diff>